<commit_message>
compelete funcs and run in a simple way again
</commit_message>
<xml_diff>
--- a/空压机概况表.xlsx
+++ b/空压机概况表.xlsx
@@ -474,7 +474,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -509,7 +509,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -610,7 +610,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -620,12 +620,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>105920</t>
+          <t>80644</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>91201</t>
+          <t>69589</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -635,7 +635,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>(105920-91201)/105920*40%*132=7.3373</t>
+          <t>(80644-69589)/80644*40%*132=7.238</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -645,12 +645,12 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>10.5713</t>
+          <t>10.472</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>(132*1.15*0.861+10.5713)/(20.3*0.861)=8.08</t>
+          <t>(132*1.15*0.8629+10.472)/(20.3*0.8629)=8.08</t>
         </is>
       </c>
     </row>
@@ -660,7 +660,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -670,12 +670,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>105920</t>
+          <t>80644</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>91201</t>
+          <t>69589</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -685,7 +685,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>(105920-91201)/105920*40%*132=7.3373</t>
+          <t>(80644-69589)/80644*40%*132=7.238</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -695,12 +695,12 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>10.5713</t>
+          <t>10.472</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>(132*1.15*0.861+10.5713)/(20.3*0.861)=8.08</t>
+          <t>(132*1.15*0.8629+10.472)/(20.3*0.8629)=8.08</t>
         </is>
       </c>
     </row>
@@ -874,14 +874,18 @@
           <t>实比功率</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>5.9</v>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>5.9</t>
+        </is>
       </c>
       <c r="C7" t="n">
         <v>8.08</v>
       </c>
-      <c r="D7" t="n">
-        <v>5.9</v>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>5.9</t>
+        </is>
       </c>
       <c r="E7" t="n">
         <v>8.08</v>
@@ -893,14 +897,18 @@
           <t>均每立方耗电</t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>0.0983</v>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>0.0983</t>
+        </is>
       </c>
       <c r="C8" t="n">
         <v>0.1347</v>
       </c>
-      <c r="D8" t="n">
-        <v>0.0983</v>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>0.0983</t>
+        </is>
       </c>
       <c r="E8" t="n">
         <v>0.1347</v>
@@ -932,16 +940,16 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>38.1027</v>
+        <v>38.1868</v>
       </c>
       <c r="C10" t="n">
-        <v>38.1027</v>
+        <v>38.1868</v>
       </c>
       <c r="D10" t="n">
-        <v>38.1027</v>
+        <v>38.1868</v>
       </c>
       <c r="E10" t="n">
-        <v>38.1027</v>
+        <v>38.1868</v>
       </c>
     </row>
     <row r="11">
@@ -951,16 +959,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>192038</v>
+        <v>192461</v>
       </c>
       <c r="C11" t="n">
-        <v>192038</v>
+        <v>192461</v>
       </c>
       <c r="D11" t="n">
-        <v>192038</v>
+        <v>192461</v>
       </c>
       <c r="E11" t="n">
-        <v>192038</v>
+        <v>192461</v>
       </c>
     </row>
     <row r="12">
@@ -970,16 +978,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>384076</v>
+        <v>384922</v>
       </c>
       <c r="C12" t="n">
-        <v>384076</v>
+        <v>384922</v>
       </c>
       <c r="D12" t="n">
-        <v>384076</v>
+        <v>384922</v>
       </c>
       <c r="E12" t="n">
-        <v>384076</v>
+        <v>384922</v>
       </c>
     </row>
   </sheetData>

</xml_diff>